<commit_message>
News and ads tests are added
</commit_message>
<xml_diff>
--- a/docs/Check_list_abw.xlsx
+++ b/docs/Check_list_abw.xlsx
@@ -156,12 +156,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -176,10 +182,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -463,7 +471,7 @@
   <dimension ref="B1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,8 +507,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E5" t="s">
+    <row r="5" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -509,8 +520,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E7" t="s">
+    <row r="7" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -519,8 +533,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
+    <row r="9" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -534,8 +551,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
+    <row r="12" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="3" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>